<commit_message>
Kalender udfyldt og synopsis opdateret
</commit_message>
<xml_diff>
--- a/Synopsis/Studiekalender (hvilket som helst år)1.xlsx
+++ b/Synopsis/Studiekalender (hvilket som helst år)1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Documents\GitHub\SynopsisTesting\Synopsis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1C5B30-5EFA-43E8-BEBB-B8D4D4FA45E9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BD0EA7-2C5D-44FC-A697-C18E15765A4E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27780" windowHeight="13260" tabRatio="788" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>MANDAG</t>
   </si>
@@ -118,6 +118,27 @@
   </si>
   <si>
     <t>Arbejde</t>
+  </si>
+  <si>
+    <t>arbejde</t>
+  </si>
+  <si>
+    <t>Research om Microsoft Test Manager (MTM)</t>
+  </si>
+  <si>
+    <t>Udforskning af MTM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Udforskning af MTM </t>
+  </si>
+  <si>
+    <t>Research om MTM</t>
+  </si>
+  <si>
+    <t>Korrektur læsning af synopsis</t>
+  </si>
+  <si>
+    <t>Tilføje eller fjerne irrelavante indhold i synopsis</t>
   </si>
 </sst>
 </file>
@@ -461,6 +482,9 @@
     <xf numFmtId="0" fontId="12" fillId="8" borderId="5" xfId="6" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="8">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -468,9 +492,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="8" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="8">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -864,8 +885,8 @@
   </sheetPr>
   <dimension ref="A1:H164"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1186,7 +1207,9 @@
       <c r="G14" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="11"/>
+      <c r="H14" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
@@ -1219,13 +1242,23 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="B16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="11"/>
+      <c r="H16" s="11" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
@@ -1258,11 +1291,21 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
+      <c r="B18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="G18" s="10"/>
       <c r="H18" s="11"/>
     </row>
@@ -1297,9 +1340,15 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
+      <c r="B20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E20" s="10" t="s">
         <v>4</v>
       </c>
@@ -1355,22 +1404,22 @@
         <f ca="1"/>
         <v>43466</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
     </row>
     <row r="24" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
     </row>
     <row r="25" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A25" s="2"/>
@@ -1623,22 +1672,22 @@
         <f ca="1"/>
         <v>43501</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
     </row>
     <row r="38" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
     </row>
     <row r="39" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A39" s="2"/>
@@ -1891,22 +1940,22 @@
         <f ca="1"/>
         <v>43529</v>
       </c>
-      <c r="D51" s="18" t="s">
+      <c r="D51" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="19"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
     </row>
     <row r="52" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
     </row>
     <row r="53" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A53" s="2"/>
@@ -2159,22 +2208,22 @@
         <f ca="1"/>
         <v>43557</v>
       </c>
-      <c r="D65" s="18" t="s">
+      <c r="D65" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E65" s="19"/>
-      <c r="F65" s="19"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="19"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="20"/>
     </row>
     <row r="66" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="18"/>
     </row>
     <row r="67" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A67" s="2"/>
@@ -2427,22 +2476,22 @@
         <f ca="1"/>
         <v>43592</v>
       </c>
-      <c r="D79" s="18" t="s">
+      <c r="D79" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E79" s="19"/>
-      <c r="F79" s="19"/>
-      <c r="G79" s="19"/>
-      <c r="H79" s="19"/>
+      <c r="E79" s="20"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="20"/>
+      <c r="H79" s="20"/>
     </row>
     <row r="80" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="10"/>
       <c r="C80" s="10"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
-      <c r="G80" s="17"/>
-      <c r="H80" s="17"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="18"/>
     </row>
     <row r="81" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A81" s="2"/>
@@ -2695,22 +2744,22 @@
         <f ca="1"/>
         <v>43620</v>
       </c>
-      <c r="D93" s="18" t="s">
+      <c r="D93" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E93" s="19"/>
-      <c r="F93" s="19"/>
-      <c r="G93" s="19"/>
-      <c r="H93" s="19"/>
+      <c r="E93" s="20"/>
+      <c r="F93" s="20"/>
+      <c r="G93" s="20"/>
+      <c r="H93" s="20"/>
     </row>
     <row r="94" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="10"/>
       <c r="C94" s="10"/>
-      <c r="D94" s="17"/>
-      <c r="E94" s="17"/>
-      <c r="F94" s="17"/>
-      <c r="G94" s="17"/>
-      <c r="H94" s="17"/>
+      <c r="D94" s="18"/>
+      <c r="E94" s="18"/>
+      <c r="F94" s="18"/>
+      <c r="G94" s="18"/>
+      <c r="H94" s="18"/>
     </row>
     <row r="95" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A95" s="2"/>
@@ -2963,22 +3012,22 @@
         <f ca="1"/>
         <v>43648</v>
       </c>
-      <c r="D107" s="18" t="s">
+      <c r="D107" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E107" s="19"/>
-      <c r="F107" s="19"/>
-      <c r="G107" s="19"/>
-      <c r="H107" s="19"/>
+      <c r="E107" s="20"/>
+      <c r="F107" s="20"/>
+      <c r="G107" s="20"/>
+      <c r="H107" s="20"/>
     </row>
     <row r="108" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B108" s="10"/>
       <c r="C108" s="10"/>
-      <c r="D108" s="17"/>
-      <c r="E108" s="17"/>
-      <c r="F108" s="17"/>
-      <c r="G108" s="17"/>
-      <c r="H108" s="17"/>
+      <c r="D108" s="18"/>
+      <c r="E108" s="18"/>
+      <c r="F108" s="18"/>
+      <c r="G108" s="18"/>
+      <c r="H108" s="18"/>
     </row>
     <row r="109" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A109" s="2"/>
@@ -3231,22 +3280,22 @@
         <f ca="1"/>
         <v>43683</v>
       </c>
-      <c r="D121" s="18" t="s">
+      <c r="D121" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E121" s="19"/>
-      <c r="F121" s="19"/>
-      <c r="G121" s="19"/>
-      <c r="H121" s="19"/>
+      <c r="E121" s="20"/>
+      <c r="F121" s="20"/>
+      <c r="G121" s="20"/>
+      <c r="H121" s="20"/>
     </row>
     <row r="122" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B122" s="10"/>
       <c r="C122" s="10"/>
-      <c r="D122" s="17"/>
-      <c r="E122" s="17"/>
-      <c r="F122" s="17"/>
-      <c r="G122" s="17"/>
-      <c r="H122" s="17"/>
+      <c r="D122" s="18"/>
+      <c r="E122" s="18"/>
+      <c r="F122" s="18"/>
+      <c r="G122" s="18"/>
+      <c r="H122" s="18"/>
     </row>
     <row r="123" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A123" s="2"/>
@@ -3499,22 +3548,22 @@
         <f ca="1"/>
         <v>43711</v>
       </c>
-      <c r="D135" s="18" t="s">
+      <c r="D135" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E135" s="19"/>
-      <c r="F135" s="19"/>
-      <c r="G135" s="19"/>
-      <c r="H135" s="19"/>
+      <c r="E135" s="20"/>
+      <c r="F135" s="20"/>
+      <c r="G135" s="20"/>
+      <c r="H135" s="20"/>
     </row>
     <row r="136" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B136" s="10"/>
       <c r="C136" s="10"/>
-      <c r="D136" s="17"/>
-      <c r="E136" s="17"/>
-      <c r="F136" s="17"/>
-      <c r="G136" s="17"/>
-      <c r="H136" s="17"/>
+      <c r="D136" s="18"/>
+      <c r="E136" s="18"/>
+      <c r="F136" s="18"/>
+      <c r="G136" s="18"/>
+      <c r="H136" s="18"/>
     </row>
     <row r="137" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B137" s="1">
@@ -3765,22 +3814,22 @@
         <f ca="1"/>
         <v>43739</v>
       </c>
-      <c r="D149" s="18" t="s">
+      <c r="D149" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E149" s="19"/>
-      <c r="F149" s="19"/>
-      <c r="G149" s="19"/>
-      <c r="H149" s="19"/>
+      <c r="E149" s="20"/>
+      <c r="F149" s="20"/>
+      <c r="G149" s="20"/>
+      <c r="H149" s="20"/>
     </row>
     <row r="150" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B150" s="10"/>
       <c r="C150" s="10"/>
-      <c r="D150" s="17"/>
-      <c r="E150" s="17"/>
-      <c r="F150" s="17"/>
-      <c r="G150" s="17"/>
-      <c r="H150" s="17"/>
+      <c r="D150" s="18"/>
+      <c r="E150" s="18"/>
+      <c r="F150" s="18"/>
+      <c r="G150" s="18"/>
+      <c r="H150" s="18"/>
     </row>
     <row r="151" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B151" s="1">
@@ -4031,35 +4080,25 @@
         <f ca="1"/>
         <v>43774</v>
       </c>
-      <c r="D163" s="18" t="s">
+      <c r="D163" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E163" s="19"/>
-      <c r="F163" s="19"/>
-      <c r="G163" s="19"/>
-      <c r="H163" s="19"/>
+      <c r="E163" s="20"/>
+      <c r="F163" s="20"/>
+      <c r="G163" s="20"/>
+      <c r="H163" s="20"/>
     </row>
     <row r="164" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B164" s="10"/>
       <c r="C164" s="10"/>
-      <c r="D164" s="17"/>
-      <c r="E164" s="17"/>
-      <c r="F164" s="17"/>
-      <c r="G164" s="17"/>
-      <c r="H164" s="17"/>
+      <c r="D164" s="18"/>
+      <c r="E164" s="18"/>
+      <c r="F164" s="18"/>
+      <c r="G164" s="18"/>
+      <c r="H164" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="D37:H37"/>
-    <mergeCell ref="D79:H79"/>
-    <mergeCell ref="D149:H149"/>
-    <mergeCell ref="D38:H38"/>
-    <mergeCell ref="D52:H52"/>
-    <mergeCell ref="D66:H66"/>
-    <mergeCell ref="D51:H51"/>
-    <mergeCell ref="D65:H65"/>
     <mergeCell ref="D164:H164"/>
     <mergeCell ref="D135:H135"/>
     <mergeCell ref="D136:H136"/>
@@ -4072,6 +4111,16 @@
     <mergeCell ref="D108:H108"/>
     <mergeCell ref="D150:H150"/>
     <mergeCell ref="D163:H163"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="D37:H37"/>
+    <mergeCell ref="D79:H79"/>
+    <mergeCell ref="D149:H149"/>
+    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="D52:H52"/>
+    <mergeCell ref="D66:H66"/>
+    <mergeCell ref="D51:H51"/>
+    <mergeCell ref="D65:H65"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:H3 B5:H5 B7:H7 B9:H9">

</xml_diff>